<commit_message>
create temp dfs for crew pairing
</commit_message>
<xml_diff>
--- a/CGinputEX.xlsx
+++ b/CGinputEX.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HyungJoon\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HyungJoon\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC748772-D183-43D4-A6DD-9397D2B03FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3F98B1-7FD9-483F-8EC9-4FA634BE5C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FD84DC62-66BF-493C-8D1A-3CFCAFBDCFE4}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="34">
-  <si>
-    <t>Flight Data</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="32">
   <si>
     <t>INDEX</t>
   </si>
@@ -66,9 +63,6 @@
   </si>
   <si>
     <t>AIRCRAFT_TYPE</t>
-  </si>
-  <si>
-    <t>Flight-COST</t>
   </si>
   <si>
     <t>F1</t>
@@ -145,7 +139,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -160,6 +154,8 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -191,7 +187,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,18 +196,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF2CC"/>
-        <bgColor rgb="FFFFF2CC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -234,43 +224,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -278,7 +231,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -288,25 +241,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="21" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -624,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{013B2EFF-E7F2-4DE5-97D7-3B028E569A0F}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -636,73 +580,84 @@
     <col min="3" max="4" width="17.625" customWidth="1"/>
     <col min="5" max="5" width="15.625" customWidth="1"/>
     <col min="6" max="9" width="17.625" customWidth="1"/>
-    <col min="10" max="10" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="9"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="C2" s="3">
+        <v>44958</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3">
+        <v>44958</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.53819444439999997</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0.16319444444444445</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3">
-        <v>44958</v>
+        <v>44959</v>
       </c>
       <c r="D3" s="4">
         <v>0.375</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F3" s="3">
-        <v>44958</v>
+        <v>44959</v>
       </c>
       <c r="G3" s="6">
         <v>0.53819444439999997</v>
@@ -711,30 +666,27 @@
         <v>0.16319444444444445</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="6">
-        <v>0.48958333329999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3">
-        <v>44959</v>
+        <v>44960</v>
       </c>
       <c r="D4" s="4">
         <v>0.375</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F4" s="3">
-        <v>44959</v>
+        <v>44960</v>
       </c>
       <c r="G4" s="6">
         <v>0.53819444439999997</v>
@@ -743,62 +695,56 @@
         <v>0.16319444444444445</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="6">
-        <v>0.48958333329999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3">
+        <v>44961</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="3">
+        <v>44961</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.78472222219999999</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3">
-        <v>44960</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.375</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="3">
-        <v>44960</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0.53819444439999997</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0.16319444444444445</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0.81597222219999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3">
-        <v>44961</v>
+        <v>44959</v>
       </c>
       <c r="D6" s="4">
         <v>0.54166666666666663</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6" s="3">
-        <v>44961</v>
+        <v>44959</v>
       </c>
       <c r="G6" s="6">
         <v>0.78472222219999999</v>
@@ -807,30 +753,27 @@
         <v>0.24305555555555555</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="6">
-        <v>0.72916666669999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3">
-        <v>44959</v>
+        <v>44960</v>
       </c>
       <c r="D7" s="4">
         <v>0.54166666666666663</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F7" s="3">
-        <v>44959</v>
+        <v>44960</v>
       </c>
       <c r="G7" s="6">
         <v>0.78472222219999999</v>
@@ -839,62 +782,56 @@
         <v>0.24305555555555555</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="6">
-        <v>1.2152777779999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3">
+        <v>44958</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="3">
+        <v>44958</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0.87152777780000001</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.16319444444444445</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="3">
-        <v>44960</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="3">
-        <v>44960</v>
-      </c>
-      <c r="G8" s="6">
-        <v>0.78472222219999999</v>
-      </c>
-      <c r="H8" s="6">
-        <v>0.24305555555555555</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="6">
-        <v>1.2152777779999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" s="3">
-        <v>44958</v>
+        <v>44962</v>
       </c>
       <c r="D9" s="4">
         <v>0.70833333333333337</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F9" s="3">
-        <v>44958</v>
+        <v>44962</v>
       </c>
       <c r="G9" s="6">
         <v>0.87152777780000001</v>
@@ -903,18 +840,15 @@
         <v>0.16319444444444445</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="6">
-        <v>0.48958333329999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C10" s="3">
         <v>44962</v>
@@ -923,7 +857,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F10" s="3">
         <v>44962</v>
@@ -935,62 +869,56 @@
         <v>0.16319444444444445</v>
       </c>
       <c r="I10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3">
+        <v>44959</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.625</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="6">
-        <v>0.81597222219999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="F11" s="3">
+        <v>44959</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.95138888889999995</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="3">
-        <v>44962</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="3">
-        <v>44962</v>
-      </c>
-      <c r="G11" s="6">
-        <v>0.87152777780000001</v>
-      </c>
-      <c r="H11" s="6">
-        <v>0.16319444444444445</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="6">
-        <v>0.81597222219999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="B12" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3">
-        <v>44959</v>
+        <v>44960</v>
       </c>
       <c r="D12" s="4">
         <v>0.625</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F12" s="3">
-        <v>44959</v>
+        <v>44960</v>
       </c>
       <c r="G12" s="6">
         <v>0.95138888889999995</v>
@@ -999,30 +927,27 @@
         <v>0.3263888888888889</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" s="6">
-        <v>0.97916666669999997</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C13" s="3">
-        <v>44960</v>
+        <v>44961</v>
       </c>
       <c r="D13" s="4">
         <v>0.625</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F13" s="3">
-        <v>44960</v>
+        <v>44961</v>
       </c>
       <c r="G13" s="6">
         <v>0.95138888889999995</v>
@@ -1031,62 +956,56 @@
         <v>0.3263888888888889</v>
       </c>
       <c r="I13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J13" s="6">
-        <v>1.6319444439999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="C14" s="3">
+        <v>44960</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="3">
+        <v>44960</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0.65972222219999999</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="3">
-        <v>44961</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0.625</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="3">
-        <v>44961</v>
-      </c>
-      <c r="G14" s="6">
-        <v>0.95138888889999995</v>
-      </c>
-      <c r="H14" s="6">
-        <v>0.3263888888888889</v>
-      </c>
-      <c r="I14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="6">
-        <v>1.6319444439999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="C15" s="3">
-        <v>44960</v>
+        <v>44962</v>
       </c>
       <c r="D15" s="4">
         <v>0.41666666666666669</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F15" s="3">
-        <v>44960</v>
+        <v>44962</v>
       </c>
       <c r="G15" s="6">
         <v>0.65972222219999999</v>
@@ -1095,18 +1014,15 @@
         <v>0.24305555555555555</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J15" s="6">
-        <v>0.72916666669999997</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C16" s="3">
         <v>44962</v>
@@ -1115,7 +1031,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F16" s="3">
         <v>44962</v>
@@ -1127,62 +1043,56 @@
         <v>0.24305555555555555</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J16" s="6">
-        <v>0.72916666669999997</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="3">
+        <v>44961</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0.625</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="3">
+        <v>44961</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0.95138888889999995</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="3">
-        <v>44962</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="3">
-        <v>44962</v>
-      </c>
-      <c r="G17" s="6">
-        <v>0.65972222219999999</v>
-      </c>
-      <c r="H17" s="6">
-        <v>0.24305555555555555</v>
-      </c>
-      <c r="I17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="6">
-        <v>1.2152777779999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="C18" s="3">
-        <v>44961</v>
+        <v>44960</v>
       </c>
       <c r="D18" s="4">
         <v>0.625</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F18" s="3">
-        <v>44961</v>
+        <v>44960</v>
       </c>
       <c r="G18" s="6">
         <v>0.95138888889999995</v>
@@ -1191,30 +1101,27 @@
         <v>0.3263888888888889</v>
       </c>
       <c r="I18" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="6">
-        <v>1.6319444439999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="C19" s="3">
-        <v>44960</v>
+        <v>44961</v>
       </c>
       <c r="D19" s="4">
         <v>0.625</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F19" s="3">
-        <v>44960</v>
+        <v>44961</v>
       </c>
       <c r="G19" s="6">
         <v>0.95138888889999995</v>
@@ -1223,48 +1130,10 @@
         <v>0.3263888888888889</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J19" s="6">
-        <v>1.6319444439999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="3">
-        <v>44961</v>
-      </c>
-      <c r="D20" s="4">
-        <v>0.625</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="3">
-        <v>44961</v>
-      </c>
-      <c r="G20" s="6">
-        <v>0.95138888889999995</v>
-      </c>
-      <c r="H20" s="6">
-        <v>0.3263888888888889</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J20" s="6">
-        <v>1.6319444439999999</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
-  </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>